<commit_message>
si esto da error ima kill myself
</commit_message>
<xml_diff>
--- a/FASE 2/BF-0041/BF-0041 Escenarios y Casos de Prueba.xlsx
+++ b/FASE 2/BF-0041/BF-0041 Escenarios y Casos de Prueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmmel\Downloads\Proyecto-PDS-BarbieFinanciera\FASE 2\BF-0041\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421A11FB-239D-4859-AF2E-9F706549B56E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72828123-6A1A-41A3-A6AF-8D40F846BF1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20520" yWindow="765" windowWidth="20640" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="72">
   <si>
     <t>Criterios de Aceptación</t>
   </si>
@@ -93,39 +93,9 @@
     <t>CP007</t>
   </si>
   <si>
-    <t>CP008</t>
-  </si>
-  <si>
-    <t>CP009</t>
-  </si>
-  <si>
-    <t>CP010</t>
-  </si>
-  <si>
-    <t>CP011</t>
-  </si>
-  <si>
-    <t>CP012</t>
-  </si>
-  <si>
-    <t>CP013</t>
-  </si>
-  <si>
     <t>CP003</t>
   </si>
   <si>
-    <t>CP014</t>
-  </si>
-  <si>
-    <t>CP015</t>
-  </si>
-  <si>
-    <t>CP016</t>
-  </si>
-  <si>
-    <t>CP017</t>
-  </si>
-  <si>
     <t>Passed</t>
   </si>
   <si>
@@ -138,9 +108,6 @@
     <t>Presupuesto visible y editable</t>
   </si>
   <si>
-    <t>Presupuesto almacenado en la base de datos</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ingresar un valor positivo como ingreso neto </t>
   </si>
   <si>
@@ -166,9 +133,6 @@
   </si>
   <si>
     <t>Editar el monto en una categoría ya guardada</t>
-  </si>
-  <si>
-    <t>Consultar un presupuesto previamente guardado</t>
   </si>
   <si>
     <t>Ingresar un valor positivo como ingreso neto mensual en el campo correspondiente y verificar que el sistema lo acepte sin mostrar errores.</t>
@@ -221,6 +185,9 @@
   <si>
     <t>Nombre de categoría: "Videojuegos"
 Monto asignado: 101</t>
+  </si>
+  <si>
+    <t>Alimentación: 300</t>
   </si>
   <si>
     <t>Categorías predefinidas:
@@ -252,18 +219,69 @@
     <t>Asignar un monto a una sola categoría de gasto que exceda el ingreso neto mensual y verificar que el sistema muestre un mensaje de error.</t>
   </si>
   <si>
+    <t>El sistema muestra un mensaje de error indicando que el monto asignado a la categoría excede el ingreso neto mensual y no permite guardar el presupuesto.</t>
+  </si>
+  <si>
     <t>Ingreso neto mensual: 1000 Categoría:
-Alquiler: 1500</t>
+Alimentacion: 1500</t>
   </si>
   <si>
     <t>1. Dirigirse a la página de creación de ingreso.
 2. Ingresar "1000" en el campo de ingreso neto mensual.
 3. Dirigirse a la página de creación de categoría.
-4. Ingresar "1500" en la categoría "Alquiler".
+4. Ingresar "1500" en la categoría "Alimentacion".
 5. Pulsar el botón de "Guardar".</t>
   </si>
   <si>
-    <t>El sistema muestra un mensaje de error indicando que el monto asignado a la categoría excede el ingreso neto mensual y no permite guardar el presupuesto.</t>
+    <t>Visualizar el presupuesto creado y verificar categorías</t>
+  </si>
+  <si>
+    <t>Visualizar el presupuesto creado y verificar que se muestren todas las categorías de gasto con los montos asignados.</t>
+  </si>
+  <si>
+    <t>El usuario ha iniciado sesión en el sistema y ha creado un presupuesto previamente.</t>
+  </si>
+  <si>
+    <t>Categorías:</t>
+  </si>
+  <si>
+    <t>1. Dirigirse a la página de creación de categoria.
+2. Ingresar "500" en el campo de la categoría predefinida "Transporte".
+3. Ingresar "300" en el campo de la categoría predefinida "Alimentación".
+4. Ingresar "100" en el campo de la categoría predefinida "Salud".
+5. Pulsar el botón de "Guardar". 6  Seleccionar "Ver Categorias"</t>
+  </si>
+  <si>
+    <t>El sistema muestra todas las categorías de gasto ingresadas en el presupuesto (Transporte, Alimentación, Salud) con sus respectivos montos.</t>
+  </si>
+  <si>
+    <t>Salud: 100</t>
+  </si>
+  <si>
+    <t>Transporte: 500</t>
+  </si>
+  <si>
+    <t>El usuario ha iniciado sesión en el sistema y tiene un presupuesto guardado.</t>
+  </si>
+  <si>
+    <t>2. Seleccionar el presupuesto que se desea editar.</t>
+  </si>
+  <si>
+    <t>3. Buscar la opción o botón para editar el monto de la categoría "Alimentación".</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Editar monto en una categoría ya guardada </t>
+  </si>
+  <si>
+    <t>Intentar editar el monto en una categoría ya guardada y verificar que el sistema permita la edición.</t>
+  </si>
+  <si>
+    <t>1. Dirigirse a la página de presupuestos guardados.
+2. Seleccionar el presupuesto que se desea editar.
+3. Buscar la opción o botón para editar el monto de la categoría "Alimentación".</t>
+  </si>
+  <si>
+    <t>El sistema debería permitir al usuario editar el monto en la categoría "Alimentación".</t>
   </si>
 </sst>
 </file>
@@ -279,13 +297,6 @@
     <font>
       <sz val="8"/>
       <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Garamond"/>
-      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -327,12 +338,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Aptos"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="0"/>
       <name val="Aptos"/>
@@ -347,6 +352,19 @@
     </font>
     <font>
       <sz val="12"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
       <name val="Aptos"/>
       <family val="2"/>
     </font>
@@ -407,147 +425,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="6">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="14"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="14"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="20"/>
-      </left>
-      <right style="thin">
-        <color indexed="20"/>
-      </right>
-      <top style="thin">
-        <color indexed="20"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="20"/>
-      </left>
-      <right style="thin">
-        <color indexed="20"/>
-      </right>
-      <top style="thin">
-        <color indexed="20"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="14"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="14"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="medium">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -604,27 +487,14 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
+      <right/>
       <top style="thin">
-        <color indexed="8"/>
+        <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top/>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -634,195 +504,42 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="9" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="9" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="8" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -830,14 +547,155 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="12" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="11" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2003,7 +1861,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D9" sqref="D9:D10"/>
@@ -2011,7 +1869,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.36328125" defaultRowHeight="14" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="4.6328125" style="13" customWidth="1"/>
+    <col min="1" max="1" width="4.6328125" style="4" customWidth="1"/>
     <col min="2" max="2" width="38.1796875" style="1" customWidth="1"/>
     <col min="3" max="3" width="5.1796875" style="1" customWidth="1"/>
     <col min="4" max="4" width="64.90625" style="1" customWidth="1"/>
@@ -2020,258 +1878,251 @@
     <col min="7" max="16384" width="16.36328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="23" customHeight="1">
-      <c r="A1" s="17"/>
-      <c r="B1" s="18" t="s">
+    <row r="1" spans="1:6" ht="23" customHeight="1">
+      <c r="A1" s="6"/>
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="34"/>
-      <c r="E1" s="18" t="s">
+      <c r="D1" s="37"/>
+      <c r="E1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="36.5" customHeight="1">
-      <c r="A2" s="41">
+    <row r="2" spans="1:6" ht="36.5" customHeight="1">
+      <c r="A2" s="44">
         <v>1</v>
       </c>
-      <c r="B2" s="38" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="16">
+      <c r="B2" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="5">
         <v>1</v>
       </c>
-      <c r="D2" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="20" t="s">
+      <c r="D2" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16" customHeight="1">
-      <c r="A3" s="42"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="41">
+    <row r="3" spans="1:6" ht="16" customHeight="1">
+      <c r="A3" s="45"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="44">
         <f>C2+1</f>
         <v>2</v>
       </c>
-      <c r="D3" s="44" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="44" t="s">
+      <c r="D3" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="24" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16" customHeight="1">
-      <c r="A4" s="43"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-    </row>
-    <row r="5" spans="1:5" ht="16" customHeight="1">
-      <c r="A5" s="26">
+    <row r="4" spans="1:6" ht="16" customHeight="1">
+      <c r="A4" s="46"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+    </row>
+    <row r="5" spans="1:6" ht="16" customHeight="1">
+      <c r="A5" s="52">
         <v>2</v>
       </c>
-      <c r="B5" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="31">
+      <c r="B5" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="33">
         <v>3</v>
       </c>
-      <c r="D5" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" s="29" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="16" customHeight="1">
-      <c r="A6" s="27"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-    </row>
-    <row r="7" spans="1:5" ht="33" customHeight="1">
-      <c r="A7" s="27"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="31">
+      <c r="D5" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="16" customHeight="1">
+      <c r="A6" s="53"/>
+      <c r="B6" s="50"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+    </row>
+    <row r="7" spans="1:6" ht="33" customHeight="1">
+      <c r="A7" s="53"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="33">
         <v>4</v>
       </c>
-      <c r="D7" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="19" t="s">
+      <c r="D7" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="25.5" hidden="1" customHeight="1">
-      <c r="A8" s="28"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="19"/>
-    </row>
-    <row r="9" spans="1:5" ht="16" customHeight="1">
-      <c r="A9" s="36">
+    <row r="8" spans="1:6" ht="25.5" hidden="1" customHeight="1">
+      <c r="A8" s="54"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" spans="1:6" ht="16" customHeight="1">
+      <c r="A9" s="39">
         <v>3</v>
       </c>
-      <c r="B9" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="51">
+      <c r="B9" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="35">
         <v>5</v>
       </c>
-      <c r="D9" s="52" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="54"/>
-    </row>
-    <row r="10" spans="1:5" ht="16" customHeight="1">
-      <c r="A10" s="37">
+      <c r="D9" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="16" customHeight="1">
+      <c r="A10" s="40">
         <f t="shared" ref="A10:A13" si="0">A9+1</f>
         <v>4</v>
       </c>
-      <c r="B10" s="35"/>
-      <c r="C10" s="51"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="54"/>
-    </row>
-    <row r="11" spans="1:5" ht="13.25" customHeight="1">
-      <c r="A11" s="46">
+      <c r="B10" s="38"/>
+      <c r="C10" s="35"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="28"/>
+    </row>
+    <row r="11" spans="1:6" ht="13.25" customHeight="1">
+      <c r="A11" s="29">
         <v>4</v>
       </c>
-      <c r="B11" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="46">
+      <c r="B11" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="29">
         <v>6</v>
       </c>
-      <c r="D11" s="47" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="59"/>
-    </row>
-    <row r="12" spans="1:5" ht="27.5" customHeight="1">
-      <c r="A12" s="46">
+      <c r="D11" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="27.5" customHeight="1">
+      <c r="A12" s="29">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B12" s="47"/>
-      <c r="C12" s="46"/>
-      <c r="D12" s="47"/>
-      <c r="E12" s="60"/>
-    </row>
-    <row r="13" spans="1:5" ht="16">
-      <c r="A13" s="46">
+      <c r="B12" s="30"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="32"/>
+    </row>
+    <row r="13" spans="1:6" ht="16">
+      <c r="A13" s="29">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B13" s="47"/>
-      <c r="C13" s="21">
+      <c r="B13" s="30"/>
+      <c r="C13" s="10">
         <v>7</v>
       </c>
-      <c r="D13" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" s="22"/>
-    </row>
-    <row r="14" spans="1:5" ht="41" customHeight="1">
-      <c r="A14" s="48">
-        <v>5</v>
-      </c>
-      <c r="B14" s="50" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="57">
-        <v>8</v>
-      </c>
-      <c r="D14" s="55" t="s">
-        <v>43</v>
-      </c>
-      <c r="E14" s="55"/>
-    </row>
-    <row r="15" spans="1:5" ht="16" hidden="1" customHeight="1">
-      <c r="A15" s="49"/>
-      <c r="B15" s="50"/>
-      <c r="C15" s="58"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
-    </row>
-    <row r="16" spans="1:5" ht="13">
-      <c r="A16" s="61"/>
-      <c r="B16" s="62"/>
-      <c r="C16" s="62"/>
-      <c r="D16" s="62"/>
-      <c r="E16" s="62"/>
-    </row>
-    <row r="17" spans="1:5" ht="12.5">
-      <c r="A17" s="63"/>
-      <c r="B17" s="64"/>
-      <c r="C17" s="64"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="64"/>
-    </row>
-    <row r="18" spans="1:5" ht="12.5">
-      <c r="A18" s="63"/>
-      <c r="B18" s="64"/>
-      <c r="C18" s="64"/>
-      <c r="D18" s="64"/>
-      <c r="E18" s="64"/>
-    </row>
-    <row r="19" spans="1:5" ht="12.5">
-      <c r="A19" s="63"/>
-      <c r="B19" s="64"/>
-      <c r="C19" s="64"/>
-      <c r="D19" s="64"/>
-      <c r="E19" s="64"/>
-    </row>
-    <row r="20" spans="1:5" ht="14" customHeight="1">
-      <c r="A20" s="63"/>
-      <c r="B20" s="64"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="64"/>
-      <c r="E20" s="64"/>
-    </row>
-    <row r="21" spans="1:5" ht="14" customHeight="1">
-      <c r="A21" s="63"/>
-      <c r="B21" s="64"/>
-      <c r="C21" s="64"/>
-      <c r="D21" s="64"/>
-      <c r="E21" s="64"/>
-    </row>
-    <row r="22" spans="1:5" ht="14" customHeight="1">
-      <c r="A22" s="63"/>
-      <c r="B22" s="64"/>
-      <c r="C22" s="64"/>
-      <c r="D22" s="64"/>
-      <c r="E22" s="64"/>
-    </row>
-    <row r="23" spans="1:5" ht="14" customHeight="1">
-      <c r="A23" s="63"/>
-      <c r="B23" s="64"/>
-      <c r="C23" s="64"/>
-      <c r="D23" s="64"/>
-      <c r="E23" s="64"/>
+      <c r="D13" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="41" customHeight="1">
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14" s="13"/>
+    </row>
+    <row r="15" spans="1:6" ht="16" hidden="1" customHeight="1">
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15" s="13"/>
+    </row>
+    <row r="16" spans="1:6" ht="12.5">
+      <c r="A16"/>
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16" s="13"/>
+    </row>
+    <row r="17" spans="1:6" ht="12.5">
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17" s="13"/>
+    </row>
+    <row r="18" spans="1:6" ht="12.5">
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18" s="13"/>
+    </row>
+    <row r="19" spans="1:6" ht="12.5">
+      <c r="A19" s="12"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+    </row>
+    <row r="20" spans="1:6" ht="14" customHeight="1">
+      <c r="A20" s="12"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+    </row>
+    <row r="21" spans="1:6" ht="14" customHeight="1">
+      <c r="A21" s="12"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+    </row>
+    <row r="22" spans="1:6" ht="14" customHeight="1">
+      <c r="A22" s="12"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+    </row>
+    <row r="23" spans="1:6" ht="14" customHeight="1">
+      <c r="A23" s="12"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="C14:C15"/>
+  <mergeCells count="23">
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="B11:B13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="C1:D1"/>
@@ -2286,6 +2137,12 @@
     <mergeCell ref="A5:A8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="C7:C8"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
     <mergeCell ref="D5:D6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2302,334 +2159,378 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomRight" activeCell="H6" sqref="A6:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="16.36328125" defaultRowHeight="14" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10" style="4" customWidth="1"/>
-    <col min="2" max="2" width="21.90625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="34.6328125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="23.6328125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="22.81640625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="44.54296875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="24.453125" style="4" customWidth="1"/>
-    <col min="8" max="9" width="16.36328125" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="16.36328125" style="4"/>
+    <col min="1" max="1" width="10" style="2" customWidth="1"/>
+    <col min="2" max="2" width="21.90625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="34.6328125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="23.6328125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.81640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="44.54296875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="24.453125" style="2" customWidth="1"/>
+    <col min="8" max="9" width="16.36328125" style="2" customWidth="1"/>
+    <col min="10" max="16384" width="16.36328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.25" customHeight="1" thickBot="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="93">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:9" ht="87">
+      <c r="A2" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="139" customHeight="1">
+      <c r="A3" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" ht="101.5">
+      <c r="A4" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4"/>
+    </row>
+    <row r="5" spans="1:9" ht="149.5" customHeight="1">
+      <c r="A5" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D5" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" s="7" t="s">
+      <c r="E5" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="109" customHeight="1">
+      <c r="A6" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G2" s="6" t="s">
+      <c r="C6" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="29" customHeight="1">
+      <c r="A7" s="56" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="62" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" s="59" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="H7" s="55" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="29" customHeight="1">
+      <c r="A8" s="57"/>
+      <c r="B8" s="62"/>
+      <c r="C8" s="55"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="F8" s="60"/>
+      <c r="G8" s="55"/>
+      <c r="H8" s="55"/>
+    </row>
+    <row r="9" spans="1:9" ht="29" customHeight="1">
+      <c r="A9" s="57"/>
+      <c r="B9" s="62"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="139" customHeight="1">
-      <c r="A3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="66" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="F9" s="60"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="55"/>
+    </row>
+    <row r="10" spans="1:9" ht="53" customHeight="1">
+      <c r="A10" s="58"/>
+      <c r="B10" s="62"/>
+      <c r="C10" s="55"/>
+      <c r="D10" s="63"/>
+      <c r="E10" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="61"/>
+      <c r="G10" s="55"/>
+      <c r="H10" s="55"/>
+    </row>
+    <row r="11" spans="1:9" ht="57.5" customHeight="1">
+      <c r="A11" s="56" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="62" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="55" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="I3" s="11"/>
-    </row>
-    <row r="4" spans="1:9" ht="108.5">
-      <c r="A4" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="66" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4"/>
-    </row>
-    <row r="5" spans="1:9" ht="149.5" customHeight="1">
-      <c r="A5" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="66" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="109" customHeight="1">
-      <c r="A6" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="67" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="F6" s="10" t="s">
+      <c r="F11" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" s="55" t="s">
+        <v>71</v>
+      </c>
+      <c r="H11" s="55" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.5">
+      <c r="A12" s="57"/>
+      <c r="B12" s="62"/>
+      <c r="C12" s="55"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="55"/>
+      <c r="F12" s="55" t="s">
         <v>66</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G12" s="55"/>
+      <c r="H12" s="55"/>
+    </row>
+    <row r="13" spans="1:9" ht="15.5">
+      <c r="A13" s="57"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="55"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="H6" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15.5">
-      <c r="A7" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="67"/>
-      <c r="C7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="15.5">
-      <c r="A8" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="67"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.5">
-      <c r="A9" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="67"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-    </row>
-    <row r="10" spans="1:9" ht="15.5">
-      <c r="A10" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="67"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-    </row>
-    <row r="11" spans="1:9" ht="109.5" customHeight="1">
-      <c r="A11" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-    </row>
-    <row r="12" spans="1:9" ht="15.5">
-      <c r="A12" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-    </row>
-    <row r="13" spans="1:9" ht="15.5">
-      <c r="A13" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="9"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
+      <c r="G13" s="55"/>
+      <c r="H13" s="55"/>
     </row>
     <row r="14" spans="1:9" ht="15.5">
-      <c r="A14" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
     </row>
     <row r="15" spans="1:9" ht="15.5">
-      <c r="A15" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="H15"/>
     </row>
     <row r="16" spans="1:9" ht="15.5">
-      <c r="A16" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
+      <c r="A16"/>
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16"/>
     </row>
     <row r="17" spans="1:8" ht="15.5">
-      <c r="A17" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
     </row>
     <row r="18" spans="1:8" ht="15.5">
-      <c r="A18" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="H18"/>
+    </row>
+    <row r="19" spans="1:8" ht="14" customHeight="1">
+      <c r="A19"/>
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
     </row>
   </sheetData>
+  <mergeCells count="15">
+    <mergeCell ref="G11:G13"/>
+    <mergeCell ref="H11:H13"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="H7:H10"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="G7:G10"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="H2:H18">
+  <conditionalFormatting sqref="H2:H13">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Failed"</formula>
     </cfRule>

</xml_diff>